<commit_message>
Fixing indicator 11.1 mappings
</commit_message>
<xml_diff>
--- a/api/src/main/resources/Template_MI_2021_v1.9.3.xlsx
+++ b/api/src/main/resources/Template_MI_2021_v1.9.3.xlsx
@@ -5540,7 +5540,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="between" stopIfTrue="1" id="{006C00B1-004D-40B6-A24A-008100C3006C}">
+          <x14:cfRule type="cellIs" priority="3" operator="between" stopIfTrue="1" id="{008C00CB-008E-4FB2-9FE6-008500650029}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -5560,7 +5560,7 @@
           <xm:sqref>G7:G51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="greaterThan" stopIfTrue="1" id="{00BE0014-00D1-4A56-8200-003F00540036}">
+          <x14:cfRule type="cellIs" priority="2" operator="greaterThan" stopIfTrue="1" id="{0059006A-003E-4672-8162-006F00C4009D}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -5579,7 +5579,7 @@
           <xm:sqref>G7:G51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="lessThan" stopIfTrue="1" id="{00F100A8-0053-4499-830A-0045009400A3}">
+          <x14:cfRule type="cellIs" priority="1" operator="lessThan" stopIfTrue="1" id="{00AA00CE-0046-42A9-BE57-00B200780014}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -5601,11 +5601,11 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0021004A-0036-48B5-A69B-008400A80086}" type="whole" allowBlank="1" error="Verifique se ao digitar não trocou o numerador pelo denominador" errorStyle="stop" errorTitle="Verificar" imeMode="noControl" operator="greaterThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{004900AD-00C7-431F-92D6-00B900E2001C}" type="whole" allowBlank="1" error="Verifique se ao digitar não trocou o numerador pelo denominador" errorStyle="stop" errorTitle="Verificar" imeMode="noControl" operator="greaterThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>XFD1</xm:f>
           </x14:formula1>
-          <xm:sqref>A1281:A1793 A1281:A3585 A1281:A5633 A1281:A7425 A1281:A12289 BI1281:GS32270 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889 BI32270:GS37889</xm:sqref>
+          <xm:sqref>A1281:A1793 A1281:A3585 A1281:A5633 A1281:A7425 A1281:A12289 DT1281:FX50843 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417 DT50843:FX60417</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8211,7 +8211,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="150" operator="between" stopIfTrue="1" id="{004E001B-00F9-4818-8DAD-004700CB00F9}">
+          <x14:cfRule type="cellIs" priority="150" operator="between" stopIfTrue="1" id="{005E006B-0087-42C1-80E3-00BC0033002D}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8231,7 +8231,7 @@
           <xm:sqref>R10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="149" operator="greaterThan" stopIfTrue="1" id="{00CF0062-0017-462C-BD30-0003005A004D}">
+          <x14:cfRule type="cellIs" priority="149" operator="greaterThan" stopIfTrue="1" id="{002D0018-00C8-4019-9DAA-005E00DA004C}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -8250,7 +8250,7 @@
           <xm:sqref>R10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="148" operator="lessThan" stopIfTrue="1" id="{00800035-003C-4FFA-8424-009300A700AB}">
+          <x14:cfRule type="cellIs" priority="148" operator="lessThan" stopIfTrue="1" id="{002C0094-0031-4110-AFE5-006300CA0041}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -8269,7 +8269,7 @@
           <xm:sqref>R10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="147" operator="between" stopIfTrue="1" id="{00E800BB-001D-44EF-B116-00D200B900E4}">
+          <x14:cfRule type="cellIs" priority="147" operator="between" stopIfTrue="1" id="{0042007C-0002-4A15-BC5E-0055004E0014}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8289,7 +8289,7 @@
           <xm:sqref>O10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="146" operator="greaterThan" stopIfTrue="1" id="{0049004F-00B3-45FC-AD26-0097000300E8}">
+          <x14:cfRule type="cellIs" priority="146" operator="greaterThan" stopIfTrue="1" id="{000C0055-008C-46C0-9922-002100380035}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -8308,7 +8308,7 @@
           <xm:sqref>O10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="145" operator="lessThan" stopIfTrue="1" id="{00160008-0050-4B6A-B1F6-00ED0053000D}">
+          <x14:cfRule type="cellIs" priority="145" operator="lessThan" stopIfTrue="1" id="{00BD00AD-00E2-477C-94AD-00CA00B30067}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -8327,7 +8327,7 @@
           <xm:sqref>O10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="144" operator="between" stopIfTrue="1" id="{00BC0072-0090-40D8-B4A3-005A009C00F7}">
+          <x14:cfRule type="cellIs" priority="144" operator="between" stopIfTrue="1" id="{005600E9-003C-4842-A741-00A7001000AC}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8347,7 +8347,7 @@
           <xm:sqref>L10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="143" operator="greaterThan" stopIfTrue="1" id="{004A0021-0012-4662-BBBE-005600450049}">
+          <x14:cfRule type="cellIs" priority="143" operator="greaterThan" stopIfTrue="1" id="{007600E2-0006-4841-817A-0089003E008A}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -8366,7 +8366,7 @@
           <xm:sqref>L10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="142" operator="lessThan" stopIfTrue="1" id="{0079005A-009B-426C-8DEE-004B00B90015}">
+          <x14:cfRule type="cellIs" priority="142" operator="lessThan" stopIfTrue="1" id="{00F7000A-00C3-4390-B139-006D0003003E}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -8385,7 +8385,7 @@
           <xm:sqref>L10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="141" operator="between" stopIfTrue="1" id="{008F006E-00BB-4098-BE0B-00B3004800EE}">
+          <x14:cfRule type="cellIs" priority="141" operator="between" stopIfTrue="1" id="{006400AF-0024-40B7-AF12-007700D50076}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8405,7 +8405,7 @@
           <xm:sqref>I10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="140" operator="greaterThan" stopIfTrue="1" id="{00A200EC-00F4-4C59-9FEB-008100C90057}">
+          <x14:cfRule type="cellIs" priority="140" operator="greaterThan" stopIfTrue="1" id="{001D00CC-000A-4993-904E-002100570034}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -8424,7 +8424,7 @@
           <xm:sqref>I10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="139" operator="lessThan" stopIfTrue="1" id="{006900E5-00FD-4B54-9656-00DB00420039}">
+          <x14:cfRule type="cellIs" priority="139" operator="lessThan" stopIfTrue="1" id="{009A0000-009E-4D5C-911C-00BC00560049}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -8443,7 +8443,7 @@
           <xm:sqref>I10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="138" operator="between" stopIfTrue="1" id="{00BA009B-00D5-4ACC-9249-007A003100B6}">
+          <x14:cfRule type="cellIs" priority="138" operator="between" stopIfTrue="1" id="{00A70029-00A3-4131-A6F7-0099006E00A2}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8463,7 +8463,7 @@
           <xm:sqref>F10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="137" operator="greaterThan" stopIfTrue="1" id="{00610044-0081-480A-9291-0012004E001D}">
+          <x14:cfRule type="cellIs" priority="137" operator="greaterThan" stopIfTrue="1" id="{00F80094-0049-42C4-97A2-009A00A00078}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -8482,7 +8482,7 @@
           <xm:sqref>F10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="136" operator="lessThan" stopIfTrue="1" id="{00F30045-007D-41BA-A79A-009100C6004A}">
+          <x14:cfRule type="cellIs" priority="136" operator="lessThan" stopIfTrue="1" id="{00080050-003B-4ABF-9F55-006F00B500A0}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -8501,7 +8501,7 @@
           <xm:sqref>F10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="135" operator="between" stopIfTrue="1" id="{00D4007D-0073-411E-8056-008E002100BF}">
+          <x14:cfRule type="cellIs" priority="135" operator="between" stopIfTrue="1" id="{004D0088-0093-44AB-9A4A-0092000D0091}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8521,7 +8521,7 @@
           <xm:sqref>GZ10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="134" operator="greaterThan" stopIfTrue="1" id="{00EA002A-0091-4ECD-A2A1-00F600F800A4}">
+          <x14:cfRule type="cellIs" priority="134" operator="greaterThan" stopIfTrue="1" id="{003D00D9-00A8-4AC4-BBC3-007F00210001}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -8540,7 +8540,7 @@
           <xm:sqref>GZ10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="133" operator="lessThan" stopIfTrue="1" id="{0008004B-00E3-4CBE-AC43-009F003D00E0}">
+          <x14:cfRule type="cellIs" priority="133" operator="lessThan" stopIfTrue="1" id="{005D0005-0001-4FBD-9055-006D00730048}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -8559,7 +8559,7 @@
           <xm:sqref>GZ10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="132" operator="between" stopIfTrue="1" id="{00190056-00F0-4E59-A8F5-00AB00DC00A9}">
+          <x14:cfRule type="cellIs" priority="132" operator="between" stopIfTrue="1" id="{0041007E-00E1-4DAF-B856-0091007400B6}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8579,7 +8579,7 @@
           <xm:sqref>GW10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="131" operator="greaterThan" stopIfTrue="1" id="{00FC0003-00AA-4358-90B0-002D00E40011}">
+          <x14:cfRule type="cellIs" priority="131" operator="greaterThan" stopIfTrue="1" id="{00A400E7-00B6-4DA3-8FB4-002E001000EE}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -8598,7 +8598,7 @@
           <xm:sqref>GW10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="130" operator="lessThan" stopIfTrue="1" id="{006B0059-0097-458B-8F61-006D00F900A2}">
+          <x14:cfRule type="cellIs" priority="130" operator="lessThan" stopIfTrue="1" id="{005800D9-00B0-470F-ACC4-00D6006700D7}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -8617,7 +8617,7 @@
           <xm:sqref>GW10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="129" operator="between" stopIfTrue="1" id="{0085009A-00A0-4ADC-A4ED-005500F800D4}">
+          <x14:cfRule type="cellIs" priority="129" operator="between" stopIfTrue="1" id="{00FD003E-0069-4647-BC5C-006400460023}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8637,7 +8637,7 @@
           <xm:sqref>GT10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="128" operator="greaterThan" stopIfTrue="1" id="{004700EF-003F-4736-A930-00E90045007D}">
+          <x14:cfRule type="cellIs" priority="128" operator="greaterThan" stopIfTrue="1" id="{009F00CE-00F0-41B0-9A29-007200CF00DD}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -8656,7 +8656,7 @@
           <xm:sqref>GT10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="127" operator="lessThan" stopIfTrue="1" id="{00690078-007A-4CC7-AB9D-0077001C0024}">
+          <x14:cfRule type="cellIs" priority="127" operator="lessThan" stopIfTrue="1" id="{008A0049-0020-41B3-91E8-003900FC0001}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -8675,7 +8675,7 @@
           <xm:sqref>GT10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="126" operator="between" stopIfTrue="1" id="{0051006A-0032-467D-9D1A-00D900E50074}">
+          <x14:cfRule type="cellIs" priority="126" operator="between" stopIfTrue="1" id="{00F300EF-00FF-45CF-9121-0026001F0087}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8695,7 +8695,7 @@
           <xm:sqref>FF10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="125" operator="greaterThan" stopIfTrue="1" id="{00DC008C-007E-4C5F-943E-00E400BF002B}">
+          <x14:cfRule type="cellIs" priority="125" operator="greaterThan" stopIfTrue="1" id="{009A0089-0011-44BD-B3AF-00D300530045}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -8714,7 +8714,7 @@
           <xm:sqref>FF10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="124" operator="lessThan" stopIfTrue="1" id="{00D90041-00A2-4DB5-863D-00B3007500C4}">
+          <x14:cfRule type="cellIs" priority="124" operator="lessThan" stopIfTrue="1" id="{00ED0030-00F5-40EC-BAE6-002700FC00E0}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -8733,7 +8733,7 @@
           <xm:sqref>FF10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="123" operator="between" stopIfTrue="1" id="{00A700EF-00CD-4D33-957C-005500B800BF}">
+          <x14:cfRule type="cellIs" priority="123" operator="between" stopIfTrue="1" id="{0011002F-00DB-4A89-835E-0092006900F2}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8753,7 +8753,7 @@
           <xm:sqref>EU10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="122" operator="greaterThan" stopIfTrue="1" id="{00260081-0010-45FB-B596-00A600C800B3}">
+          <x14:cfRule type="cellIs" priority="122" operator="greaterThan" stopIfTrue="1" id="{009B00BD-0097-4D55-832B-00A8005600FA}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -8772,7 +8772,7 @@
           <xm:sqref>EU10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="121" operator="lessThan" stopIfTrue="1" id="{00A8000B-00B9-41E4-B72F-002D006500CF}">
+          <x14:cfRule type="cellIs" priority="121" operator="lessThan" stopIfTrue="1" id="{00820042-00B1-42A2-9CEE-0027009000EA}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -8791,7 +8791,7 @@
           <xm:sqref>EU10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="120" operator="between" stopIfTrue="1" id="{001F00BD-00E3-4260-84AD-00A200BE002F}">
+          <x14:cfRule type="cellIs" priority="120" operator="between" stopIfTrue="1" id="{00510087-0043-445F-B3DE-0013006900AD}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8811,7 +8811,7 @@
           <xm:sqref>FE10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="119" operator="greaterThan" stopIfTrue="1" id="{00920076-0095-4BDF-A56E-00A50012009C}">
+          <x14:cfRule type="cellIs" priority="119" operator="greaterThan" stopIfTrue="1" id="{00EE0047-0025-4AF4-9D53-00F6001900AC}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -8830,7 +8830,7 @@
           <xm:sqref>FE10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="118" operator="lessThan" stopIfTrue="1" id="{00FB007E-0044-4E2C-8098-00C2001C005D}">
+          <x14:cfRule type="cellIs" priority="118" operator="lessThan" stopIfTrue="1" id="{0070006C-0075-4686-AB9A-00B800EF007B}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -8849,7 +8849,7 @@
           <xm:sqref>FE10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="117" operator="between" stopIfTrue="1" id="{00940035-0034-4C65-85D4-002900AB00A9}">
+          <x14:cfRule type="cellIs" priority="117" operator="between" stopIfTrue="1" id="{00F1002A-005A-4944-8279-001800930006}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8869,7 +8869,7 @@
           <xm:sqref>FD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="116" operator="greaterThan" stopIfTrue="1" id="{00570072-0035-4ABB-AECD-007800D700F2}">
+          <x14:cfRule type="cellIs" priority="116" operator="greaterThan" stopIfTrue="1" id="{002E0073-0012-4881-AE97-008B003E00C3}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -8888,7 +8888,7 @@
           <xm:sqref>FD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="115" operator="lessThan" stopIfTrue="1" id="{000A00B9-009C-44AD-BB36-002600180047}">
+          <x14:cfRule type="cellIs" priority="115" operator="lessThan" stopIfTrue="1" id="{000A000D-00AB-478F-B1AF-00640069002B}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -8907,7 +8907,7 @@
           <xm:sqref>FD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="114" operator="between" stopIfTrue="1" id="{006900DF-00E1-4CBF-8DDF-0063007B00B8}">
+          <x14:cfRule type="cellIs" priority="114" operator="between" stopIfTrue="1" id="{00410090-0047-403B-A173-00DB00C6009A}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8927,7 +8927,7 @@
           <xm:sqref>FG10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="113" operator="greaterThan" stopIfTrue="1" id="{002F0086-002C-4C3D-8644-00F60008008D}">
+          <x14:cfRule type="cellIs" priority="113" operator="greaterThan" stopIfTrue="1" id="{00C60011-0014-4002-B073-00E900A800DB}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -8946,7 +8946,7 @@
           <xm:sqref>FG10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="112" operator="lessThan" stopIfTrue="1" id="{007A0015-00F5-4E33-BFE1-008200FE0003}">
+          <x14:cfRule type="cellIs" priority="112" operator="lessThan" stopIfTrue="1" id="{00D90001-005C-46AE-BE2D-00E8009C0052}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -8965,7 +8965,7 @@
           <xm:sqref>FG10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="111" operator="between" stopIfTrue="1" id="{008F00C4-0059-4DD7-96EB-00A0003B000D}">
+          <x14:cfRule type="cellIs" priority="111" operator="between" stopIfTrue="1" id="{00AA005F-0005-4910-A240-00F8006500C5}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -8985,7 +8985,7 @@
           <xm:sqref>DL10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="110" operator="greaterThan" stopIfTrue="1" id="{009600FD-0052-4A09-B327-0073002700D5}">
+          <x14:cfRule type="cellIs" priority="110" operator="greaterThan" stopIfTrue="1" id="{005D0048-005B-4582-B2D5-00CA003A00CB}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9004,7 +9004,7 @@
           <xm:sqref>DL10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="109" operator="lessThan" stopIfTrue="1" id="{002300C7-000E-4420-AFE8-008800F4005B}">
+          <x14:cfRule type="cellIs" priority="109" operator="lessThan" stopIfTrue="1" id="{009800CC-008D-4F46-B15B-007C00320003}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9023,7 +9023,7 @@
           <xm:sqref>DL10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="108" operator="between" stopIfTrue="1" id="{004C00B9-00F7-463F-97D6-00E2004A000C}">
+          <x14:cfRule type="cellIs" priority="108" operator="between" stopIfTrue="1" id="{00D600B0-006D-4510-BC32-006B00B40029}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9043,7 +9043,7 @@
           <xm:sqref>EP10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="107" operator="greaterThan" stopIfTrue="1" id="{0088009A-00CA-48B3-BB0A-000600590033}">
+          <x14:cfRule type="cellIs" priority="107" operator="greaterThan" stopIfTrue="1" id="{0079008D-0089-4DAE-8E61-002A00A800D2}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9062,7 +9062,7 @@
           <xm:sqref>EP10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="106" operator="lessThan" stopIfTrue="1" id="{00BB0091-001A-4A60-8685-001C000D00F2}">
+          <x14:cfRule type="cellIs" priority="106" operator="lessThan" stopIfTrue="1" id="{00B600A3-00C9-4FB3-9E8C-0080005800C4}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9081,7 +9081,7 @@
           <xm:sqref>EP10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="105" operator="between" stopIfTrue="1" id="{00330051-001A-4127-8853-00530019000E}">
+          <x14:cfRule type="cellIs" priority="105" operator="between" stopIfTrue="1" id="{00D600D9-0088-4EAD-A09D-00BC001F00FB}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9101,7 +9101,7 @@
           <xm:sqref>EF10:EG10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="104" operator="greaterThan" stopIfTrue="1" id="{005E00EF-002B-4C2B-9FDD-007200330064}">
+          <x14:cfRule type="cellIs" priority="104" operator="greaterThan" stopIfTrue="1" id="{00840023-005E-48B1-A799-00AE0044003D}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9120,7 +9120,7 @@
           <xm:sqref>EF10:EG10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="103" operator="lessThan" stopIfTrue="1" id="{00B200BF-0002-4AC0-9604-006800F50084}">
+          <x14:cfRule type="cellIs" priority="103" operator="lessThan" stopIfTrue="1" id="{009B002E-00F4-42D7-B6D9-0067004E0007}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9139,7 +9139,7 @@
           <xm:sqref>EF10:EG10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="102" operator="between" stopIfTrue="1" id="{0004002B-003E-4DF6-A86F-00AD00DC0010}">
+          <x14:cfRule type="cellIs" priority="102" operator="between" stopIfTrue="1" id="{007300B6-0084-4D78-A216-00E100AF004C}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9159,7 +9159,7 @@
           <xm:sqref>DM10:DN10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="101" operator="greaterThan" stopIfTrue="1" id="{00FD00B1-0083-4B98-85D2-0032007E0057}">
+          <x14:cfRule type="cellIs" priority="101" operator="greaterThan" stopIfTrue="1" id="{00380027-008D-43FB-8582-00B4007200A4}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9178,7 +9178,7 @@
           <xm:sqref>DM10:DN10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="100" operator="lessThan" stopIfTrue="1" id="{00D20040-0090-444E-A558-00A0002300B7}">
+          <x14:cfRule type="cellIs" priority="100" operator="lessThan" stopIfTrue="1" id="{003B0007-00A9-4934-94C9-008500D500D1}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9197,7 +9197,7 @@
           <xm:sqref>DM10:DN10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="99" operator="between" stopIfTrue="1" id="{00BB00F7-00C9-4EAB-B149-000A00A80085}">
+          <x14:cfRule type="cellIs" priority="99" operator="between" stopIfTrue="1" id="{00AF006A-001E-4E62-A23E-00F0006E00F7}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9217,7 +9217,7 @@
           <xm:sqref>EH10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="98" operator="greaterThan" stopIfTrue="1" id="{0039009F-0056-47E2-A170-002B00A400A5}">
+          <x14:cfRule type="cellIs" priority="98" operator="greaterThan" stopIfTrue="1" id="{007400B8-0064-40D0-BBD8-00AE004B00CD}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9236,7 +9236,7 @@
           <xm:sqref>EH10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="97" operator="lessThan" stopIfTrue="1" id="{000C0069-0068-4E55-9B58-00B700D100D4}">
+          <x14:cfRule type="cellIs" priority="97" operator="lessThan" stopIfTrue="1" id="{00CB000A-00EC-40F9-A5BD-00C5006C00D7}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9255,7 +9255,7 @@
           <xm:sqref>EH10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="96" operator="between" stopIfTrue="1" id="{001F00AC-002E-409A-82BB-00EE000A008B}">
+          <x14:cfRule type="cellIs" priority="96" operator="between" stopIfTrue="1" id="{002F0031-0055-4838-9A6E-004E008F00C2}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9275,7 +9275,7 @@
           <xm:sqref>EQ10:ER10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="95" operator="greaterThan" stopIfTrue="1" id="{0025003C-005C-477F-89D3-006500B600D6}">
+          <x14:cfRule type="cellIs" priority="95" operator="greaterThan" stopIfTrue="1" id="{000D00D4-0068-4F3F-A361-00FE002100C3}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9294,7 +9294,7 @@
           <xm:sqref>EQ10:ER10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="94" operator="lessThan" stopIfTrue="1" id="{0091001D-0060-4CBD-B5AB-00C000670001}">
+          <x14:cfRule type="cellIs" priority="94" operator="lessThan" stopIfTrue="1" id="{00BE00F7-000B-4FE7-A024-0052008300B3}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9313,7 +9313,7 @@
           <xm:sqref>EQ10:ER10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="93" operator="between" stopIfTrue="1" id="{00C80092-0067-463D-9A6D-00FE00D40031}">
+          <x14:cfRule type="cellIs" priority="93" operator="between" stopIfTrue="1" id="{006B003C-009A-45A9-844C-009000BC0077}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9333,7 +9333,7 @@
           <xm:sqref>DB10:DC10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="92" operator="greaterThan" stopIfTrue="1" id="{0085002B-004E-4EAE-BB35-00A200800071}">
+          <x14:cfRule type="cellIs" priority="92" operator="greaterThan" stopIfTrue="1" id="{00A20092-0092-4ADF-B6B6-0061008A002A}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9352,7 +9352,7 @@
           <xm:sqref>DB10:DC10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="91" operator="lessThan" stopIfTrue="1" id="{00ED00A8-0043-41EC-BBC5-000600900004}">
+          <x14:cfRule type="cellIs" priority="91" operator="lessThan" stopIfTrue="1" id="{00AB00FF-009C-45F8-BA06-00C7009000B3}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9371,7 +9371,7 @@
           <xm:sqref>DB10:DC10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="90" operator="between" stopIfTrue="1" id="{00FA00F9-00EE-43C9-B8E5-00D1006900AA}">
+          <x14:cfRule type="cellIs" priority="90" operator="between" stopIfTrue="1" id="{00D400C5-0026-4A5D-8A2F-002F0052001F}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9391,7 +9391,7 @@
           <xm:sqref>DE10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="89" operator="greaterThan" stopIfTrue="1" id="{00D000C8-0013-465F-A493-008100F700C2}">
+          <x14:cfRule type="cellIs" priority="89" operator="greaterThan" stopIfTrue="1" id="{001A00F7-0081-42F0-83ED-0045005500E3}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9410,7 +9410,7 @@
           <xm:sqref>DE10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="88" operator="lessThan" stopIfTrue="1" id="{00BC00C7-0007-40B8-8BC5-00DC006A0094}">
+          <x14:cfRule type="cellIs" priority="88" operator="lessThan" stopIfTrue="1" id="{009D008C-000E-41EA-BB76-007C0058000B}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9429,7 +9429,7 @@
           <xm:sqref>DE10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="87" operator="between" stopIfTrue="1" id="{00BB0071-00E8-4511-938E-003F00CE0097}">
+          <x14:cfRule type="cellIs" priority="87" operator="between" stopIfTrue="1" id="{000F0042-008F-46F0-8AB7-008F0054009E}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9449,7 +9449,7 @@
           <xm:sqref>DD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="86" operator="greaterThan" stopIfTrue="1" id="{00F20014-001D-4730-8072-002300420051}">
+          <x14:cfRule type="cellIs" priority="86" operator="greaterThan" stopIfTrue="1" id="{007A0012-00DA-4C97-891F-0015007100E1}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9468,7 +9468,7 @@
           <xm:sqref>DD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="85" operator="lessThan" stopIfTrue="1" id="{003D0044-00BA-41A9-A7C5-00F200950014}">
+          <x14:cfRule type="cellIs" priority="85" operator="lessThan" stopIfTrue="1" id="{00E5003A-00FD-4BD9-A2BC-000600580030}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9487,7 +9487,7 @@
           <xm:sqref>DD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="84" operator="between" stopIfTrue="1" id="{00BE0098-0047-4B27-B5C4-007F00200024}">
+          <x14:cfRule type="cellIs" priority="84" operator="between" stopIfTrue="1" id="{006300DC-005C-4BC5-9EBD-00CF00B60055}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9507,7 +9507,7 @@
           <xm:sqref>EE10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="83" operator="greaterThan" stopIfTrue="1" id="{001000E1-00B2-43BF-8522-004100D70015}">
+          <x14:cfRule type="cellIs" priority="83" operator="greaterThan" stopIfTrue="1" id="{00DC00AF-003C-4FFB-92F1-00FA006C00B0}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9526,7 +9526,7 @@
           <xm:sqref>EE10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="82" operator="lessThan" stopIfTrue="1" id="{00360017-003F-4022-9882-002A000500F4}">
+          <x14:cfRule type="cellIs" priority="82" operator="lessThan" stopIfTrue="1" id="{00CF00BF-002C-4E9F-A238-001A00C400AD}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9545,7 +9545,7 @@
           <xm:sqref>EE10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="81" operator="between" stopIfTrue="1" id="{00E700BA-00EE-47C3-84AE-00AA000900D4}">
+          <x14:cfRule type="cellIs" priority="81" operator="between" stopIfTrue="1" id="{00180043-0029-46C3-8493-00EF00C50084}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9565,7 +9565,7 @@
           <xm:sqref>EI10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="80" operator="greaterThan" stopIfTrue="1" id="{009600F3-005B-4A81-B4F7-00C3003A000E}">
+          <x14:cfRule type="cellIs" priority="80" operator="greaterThan" stopIfTrue="1" id="{001E0008-0034-486E-9BE3-0058001200DF}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9584,7 +9584,7 @@
           <xm:sqref>EI10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="79" operator="lessThan" stopIfTrue="1" id="{00DB0002-009D-41E7-BDD6-00BC00340032}">
+          <x14:cfRule type="cellIs" priority="79" operator="lessThan" stopIfTrue="1" id="{00EB0077-006D-4C3E-8E64-00BE000200A0}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9603,7 +9603,7 @@
           <xm:sqref>EI10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="78" operator="between" stopIfTrue="1" id="{004000FB-0017-4A6C-8EDF-0000002D00A2}">
+          <x14:cfRule type="cellIs" priority="78" operator="between" stopIfTrue="1" id="{004200A0-00EE-46BE-BCD0-002F00910032}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9623,7 +9623,7 @@
           <xm:sqref>DA10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="77" operator="greaterThan" stopIfTrue="1" id="{00A100CA-0078-4E93-91E4-00BE00A50020}">
+          <x14:cfRule type="cellIs" priority="77" operator="greaterThan" stopIfTrue="1" id="{0097008F-00E3-4DB8-88D7-00A0008F00B4}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9642,7 +9642,7 @@
           <xm:sqref>DA10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="76" operator="lessThan" stopIfTrue="1" id="{001A00C9-00C9-45E8-837D-00D6008D00B2}">
+          <x14:cfRule type="cellIs" priority="76" operator="lessThan" stopIfTrue="1" id="{00BC0083-0044-4A1C-BF1F-003C00E700F6}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9661,7 +9661,7 @@
           <xm:sqref>DA10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="75" operator="between" stopIfTrue="1" id="{00C500C0-000F-4823-9886-000C008500FD}">
+          <x14:cfRule type="cellIs" priority="75" operator="between" stopIfTrue="1" id="{00E1006F-00CF-49AF-8450-005800410046}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9681,7 +9681,7 @@
           <xm:sqref>DS10:DT10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="74" operator="greaterThan" stopIfTrue="1" id="{00F700E8-0085-47D7-964E-008A00C0003C}">
+          <x14:cfRule type="cellIs" priority="74" operator="greaterThan" stopIfTrue="1" id="{00410061-0052-448D-971A-00B2009E0061}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9700,7 +9700,7 @@
           <xm:sqref>DS10:DT10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="73" operator="lessThan" stopIfTrue="1" id="{00D1005E-00A4-411F-ABB9-00DA00A6002A}">
+          <x14:cfRule type="cellIs" priority="73" operator="lessThan" stopIfTrue="1" id="{00DB0030-0047-41E5-BD40-00B8000200E1}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9719,7 +9719,7 @@
           <xm:sqref>DS10:DT10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="72" operator="between" stopIfTrue="1" id="{00FA0033-00CE-43FD-99E3-000500340031}">
+          <x14:cfRule type="cellIs" priority="72" operator="between" stopIfTrue="1" id="{00F60007-00C3-4EB0-9C73-0040006C002F}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9739,7 +9739,7 @@
           <xm:sqref>CM10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="71" operator="greaterThan" stopIfTrue="1" id="{008B003C-009F-4A4F-8FFC-00DF00400054}">
+          <x14:cfRule type="cellIs" priority="71" operator="greaterThan" stopIfTrue="1" id="{00900094-00E9-462F-8E5F-007A005F0004}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9758,7 +9758,7 @@
           <xm:sqref>CM10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="70" operator="lessThan" stopIfTrue="1" id="{0075002D-001B-404B-843A-003300C6005F}">
+          <x14:cfRule type="cellIs" priority="70" operator="lessThan" stopIfTrue="1" id="{00790056-0010-4098-86BE-00AF00460088}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9777,7 +9777,7 @@
           <xm:sqref>CM10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="69" operator="between" stopIfTrue="1" id="{00DC00B2-0090-4FAB-B88B-0032000700C2}">
+          <x14:cfRule type="cellIs" priority="69" operator="between" stopIfTrue="1" id="{008400D3-0043-4655-BA4F-0012000E0012}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9797,7 +9797,7 @@
           <xm:sqref>CP10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="68" operator="greaterThan" stopIfTrue="1" id="{00DA00BC-0028-4B86-8D06-00F500B700C4}">
+          <x14:cfRule type="cellIs" priority="68" operator="greaterThan" stopIfTrue="1" id="{00DB0056-00D7-47D6-BC17-00CF001300AF}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9816,7 +9816,7 @@
           <xm:sqref>CP10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="67" operator="lessThan" stopIfTrue="1" id="{00990042-008D-483A-AF47-0051009B0068}">
+          <x14:cfRule type="cellIs" priority="67" operator="lessThan" stopIfTrue="1" id="{004200F5-0023-40BA-85E2-008E00D10036}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9835,7 +9835,7 @@
           <xm:sqref>CP10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="66" operator="between" stopIfTrue="1" id="{00530015-00FC-4391-B7F2-00CF00750054}">
+          <x14:cfRule type="cellIs" priority="66" operator="between" stopIfTrue="1" id="{00C7007B-00AD-4CB5-85DA-005700A40069}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9855,7 +9855,7 @@
           <xm:sqref>CO10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="65" operator="greaterThan" stopIfTrue="1" id="{009C008A-00E6-49D8-9F1A-003400470003}">
+          <x14:cfRule type="cellIs" priority="65" operator="greaterThan" stopIfTrue="1" id="{00800095-0093-47D1-BF69-00BF008E00BB}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9874,7 +9874,7 @@
           <xm:sqref>CO10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="64" operator="lessThan" stopIfTrue="1" id="{001000FE-001A-48A7-AD0E-005E007F009E}">
+          <x14:cfRule type="cellIs" priority="64" operator="lessThan" stopIfTrue="1" id="{00720058-0037-423C-85BB-00E0006500A6}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9893,7 +9893,7 @@
           <xm:sqref>CO10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="63" operator="between" stopIfTrue="1" id="{00300088-000A-43DC-9A81-00C7004F00B5}">
+          <x14:cfRule type="cellIs" priority="63" operator="between" stopIfTrue="1" id="{00730005-00CD-4809-B083-00D800E60008}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9913,7 +9913,7 @@
           <xm:sqref>CN10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="62" operator="greaterThan" stopIfTrue="1" id="{00560063-00E5-4F53-AF90-00D00057007F}">
+          <x14:cfRule type="cellIs" priority="62" operator="greaterThan" stopIfTrue="1" id="{00C500EE-00F0-440A-AB47-0075005C0072}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9932,7 +9932,7 @@
           <xm:sqref>CN10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="61" operator="lessThan" stopIfTrue="1" id="{001C00A1-008E-4B7E-BFC9-00040097002C}">
+          <x14:cfRule type="cellIs" priority="61" operator="lessThan" stopIfTrue="1" id="{00E700D0-006C-4241-BD46-00D600AE007E}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -9951,7 +9951,7 @@
           <xm:sqref>CN10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="60" operator="between" stopIfTrue="1" id="{00CE00C4-003E-4E19-A164-004000FF000D}">
+          <x14:cfRule type="cellIs" priority="60" operator="between" stopIfTrue="1" id="{00EF007F-00BC-42E7-A851-006400B000D1}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -9971,7 +9971,7 @@
           <xm:sqref>CA10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="59" operator="greaterThan" stopIfTrue="1" id="{0015009A-0045-4096-AE97-00BD008C008D}">
+          <x14:cfRule type="cellIs" priority="59" operator="greaterThan" stopIfTrue="1" id="{0097001F-00B7-4525-9C03-00B2005700A3}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -9990,7 +9990,7 @@
           <xm:sqref>CA10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="58" operator="lessThan" stopIfTrue="1" id="{007B0045-0089-454F-96ED-0026006A009C}">
+          <x14:cfRule type="cellIs" priority="58" operator="lessThan" stopIfTrue="1" id="{000300E3-00AC-4A85-9B73-00BE00940013}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10009,7 +10009,7 @@
           <xm:sqref>CA10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="57" operator="between" stopIfTrue="1" id="{00E400BB-0021-45D7-A3E6-008000490021}">
+          <x14:cfRule type="cellIs" priority="57" operator="between" stopIfTrue="1" id="{00F60083-0023-4525-B0EC-005300B9005A}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10029,7 +10029,7 @@
           <xm:sqref>CD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="56" operator="greaterThan" stopIfTrue="1" id="{00C60007-005D-4C39-BB3D-009800FB0020}">
+          <x14:cfRule type="cellIs" priority="56" operator="greaterThan" stopIfTrue="1" id="{004700AA-0083-43A4-9A24-000300E700D3}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10048,7 +10048,7 @@
           <xm:sqref>CD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="55" operator="lessThan" stopIfTrue="1" id="{00A50094-00C9-4809-8420-002F00C400E9}">
+          <x14:cfRule type="cellIs" priority="55" operator="lessThan" stopIfTrue="1" id="{00270096-0013-4C13-8946-00F3005C00DA}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10067,7 +10067,7 @@
           <xm:sqref>CD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="54" operator="between" stopIfTrue="1" id="{006500FE-00D9-4A44-AFF0-009400BA0033}">
+          <x14:cfRule type="cellIs" priority="54" operator="between" stopIfTrue="1" id="{005B0030-0027-4101-AE67-0044005400A7}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10087,7 +10087,7 @@
           <xm:sqref>CC10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="53" operator="greaterThan" stopIfTrue="1" id="{00BF00DD-00BF-489F-88DF-0004007E0022}">
+          <x14:cfRule type="cellIs" priority="53" operator="greaterThan" stopIfTrue="1" id="{007900FD-007A-4EA6-9288-00F7008300E1}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10106,7 +10106,7 @@
           <xm:sqref>CC10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="52" operator="lessThan" stopIfTrue="1" id="{00BB00B9-00FF-48D2-9800-00F8007500BA}">
+          <x14:cfRule type="cellIs" priority="52" operator="lessThan" stopIfTrue="1" id="{005E004C-00DF-4483-8569-003400000061}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10125,7 +10125,7 @@
           <xm:sqref>CC10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="51" operator="between" stopIfTrue="1" id="{00E50071-00CF-41B2-A341-003A00E800C3}">
+          <x14:cfRule type="cellIs" priority="51" operator="between" stopIfTrue="1" id="{00FA0076-00F4-4C53-87F8-005D0040003B}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10145,7 +10145,7 @@
           <xm:sqref>CB10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="50" operator="greaterThan" stopIfTrue="1" id="{00000032-0066-44DE-A7A3-006800050089}">
+          <x14:cfRule type="cellIs" priority="50" operator="greaterThan" stopIfTrue="1" id="{00C300A5-0057-4CE2-A105-002700BA0048}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10164,7 +10164,7 @@
           <xm:sqref>CB10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="49" operator="lessThan" stopIfTrue="1" id="{00AF0042-00D6-4FF5-B12A-00F9003600E4}">
+          <x14:cfRule type="cellIs" priority="49" operator="lessThan" stopIfTrue="1" id="{007700F9-00C6-4716-BC53-00C9009C00DA}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10183,7 +10183,7 @@
           <xm:sqref>CB10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="48" operator="between" stopIfTrue="1" id="{00FC00D9-005B-4F39-AA8D-00A2003A004B}">
+          <x14:cfRule type="cellIs" priority="48" operator="between" stopIfTrue="1" id="{004800A8-00C9-4F0D-89E6-007D002E00C7}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10203,7 +10203,7 @@
           <xm:sqref>BO10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="47" operator="greaterThan" stopIfTrue="1" id="{006C00DB-0039-4DE3-A9C5-00C800140044}">
+          <x14:cfRule type="cellIs" priority="47" operator="greaterThan" stopIfTrue="1" id="{00420057-000D-40FA-8E21-009700060009}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10222,7 +10222,7 @@
           <xm:sqref>BO10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="46" operator="lessThan" stopIfTrue="1" id="{008D001C-006C-4BA9-B586-003A0043003E}">
+          <x14:cfRule type="cellIs" priority="46" operator="lessThan" stopIfTrue="1" id="{00AF006D-0031-4AD5-BFE2-008C007E00C8}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10241,7 +10241,7 @@
           <xm:sqref>BO10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="45" operator="between" stopIfTrue="1" id="{00360048-0052-47EB-B4C7-0010001500A3}">
+          <x14:cfRule type="cellIs" priority="45" operator="between" stopIfTrue="1" id="{00C4005A-0028-47FD-8DC5-002F003600CD}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10261,7 +10261,7 @@
           <xm:sqref>BR10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="44" operator="greaterThan" stopIfTrue="1" id="{008A00C1-002E-4546-B040-005400EA008C}">
+          <x14:cfRule type="cellIs" priority="44" operator="greaterThan" stopIfTrue="1" id="{00AA00AC-00B7-4AA1-8B90-000E00D70056}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10280,7 +10280,7 @@
           <xm:sqref>BR10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="43" operator="lessThan" stopIfTrue="1" id="{00000091-005B-4EC2-A8EB-008000890042}">
+          <x14:cfRule type="cellIs" priority="43" operator="lessThan" stopIfTrue="1" id="{001900F9-005E-4C51-806C-0007004300BD}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10299,7 +10299,7 @@
           <xm:sqref>BR10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="42" operator="between" stopIfTrue="1" id="{00DB00D6-0038-4C38-85AB-001C00CB009F}">
+          <x14:cfRule type="cellIs" priority="42" operator="between" stopIfTrue="1" id="{00830060-0030-43B6-AA06-00C3008500DC}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10319,7 +10319,7 @@
           <xm:sqref>BQ10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="41" operator="greaterThan" stopIfTrue="1" id="{00C5006F-00BB-4D39-BD43-007300E6004D}">
+          <x14:cfRule type="cellIs" priority="41" operator="greaterThan" stopIfTrue="1" id="{000E0027-00C1-43B7-8279-0066008F0066}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10338,7 +10338,7 @@
           <xm:sqref>BQ10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="40" operator="lessThan" stopIfTrue="1" id="{00330076-004C-4BF1-A389-008B00C300A6}">
+          <x14:cfRule type="cellIs" priority="40" operator="lessThan" stopIfTrue="1" id="{00AA00E4-001D-48ED-B26C-007100360098}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10357,7 +10357,7 @@
           <xm:sqref>BQ10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="39" operator="between" stopIfTrue="1" id="{00F00099-00EA-4E51-9A66-005800F600D6}">
+          <x14:cfRule type="cellIs" priority="39" operator="between" stopIfTrue="1" id="{002500CB-005A-4549-B664-006100EB0061}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10377,7 +10377,7 @@
           <xm:sqref>BP10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="38" operator="greaterThan" stopIfTrue="1" id="{003B00C8-000F-4FEE-AA32-003900B500B5}">
+          <x14:cfRule type="cellIs" priority="38" operator="greaterThan" stopIfTrue="1" id="{0024001A-0036-4FBE-AB37-00D6008E00E0}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10396,7 +10396,7 @@
           <xm:sqref>BP10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="37" operator="lessThan" stopIfTrue="1" id="{009D00F4-00E3-40F7-A071-0074003C00F5}">
+          <x14:cfRule type="cellIs" priority="37" operator="lessThan" stopIfTrue="1" id="{00DA008A-00AF-4041-89D6-0088008000C5}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10415,7 +10415,7 @@
           <xm:sqref>BP10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="36" operator="between" stopIfTrue="1" id="{00A100CB-00FF-46CB-A17B-0089007F00A6}">
+          <x14:cfRule type="cellIs" priority="36" operator="between" stopIfTrue="1" id="{007A007C-00F7-4D19-AD5A-001300FC00E5}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10435,7 +10435,7 @@
           <xm:sqref>BB10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="35" operator="greaterThan" stopIfTrue="1" id="{00C30037-00D3-450E-8F28-003A002400F5}">
+          <x14:cfRule type="cellIs" priority="35" operator="greaterThan" stopIfTrue="1" id="{00180050-00F7-4238-AE46-002C00DD00E2}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10454,7 +10454,7 @@
           <xm:sqref>BB10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="34" operator="lessThan" stopIfTrue="1" id="{007500B2-0079-4A7F-B590-00B100700088}">
+          <x14:cfRule type="cellIs" priority="34" operator="lessThan" stopIfTrue="1" id="{00210068-00C8-4E5C-8F35-00AE00260085}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10473,7 +10473,7 @@
           <xm:sqref>BB10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="33" operator="between" stopIfTrue="1" id="{00AF004A-0097-4909-8096-00A3002600B5}">
+          <x14:cfRule type="cellIs" priority="33" operator="between" stopIfTrue="1" id="{00850064-0028-449F-BBB7-009E00F00049}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10493,7 +10493,7 @@
           <xm:sqref>BF10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="32" operator="greaterThan" stopIfTrue="1" id="{00C90083-0013-48D3-9256-004700D40016}">
+          <x14:cfRule type="cellIs" priority="32" operator="greaterThan" stopIfTrue="1" id="{005200B8-00D4-4E6F-A321-005700780024}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10512,7 +10512,7 @@
           <xm:sqref>BF10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="31" operator="lessThan" stopIfTrue="1" id="{00190008-0047-4C90-B1F3-001000BD0037}">
+          <x14:cfRule type="cellIs" priority="31" operator="lessThan" stopIfTrue="1" id="{00620001-00CE-48DC-B4ED-007D00E500B1}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10531,7 +10531,7 @@
           <xm:sqref>BF10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="30" operator="between" stopIfTrue="1" id="{00E800AC-0041-4933-936D-008F00B900B8}">
+          <x14:cfRule type="cellIs" priority="30" operator="between" stopIfTrue="1" id="{00C10072-000D-4478-8C8B-00A500B000F4}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10551,7 +10551,7 @@
           <xm:sqref>BE10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="29" operator="greaterThan" stopIfTrue="1" id="{00FE0020-00E0-4EE7-BE39-009500500067}">
+          <x14:cfRule type="cellIs" priority="29" operator="greaterThan" stopIfTrue="1" id="{005D0022-00B0-4339-B440-004C001000FD}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10570,7 +10570,7 @@
           <xm:sqref>BE10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="28" operator="lessThan" stopIfTrue="1" id="{00B10050-0063-417A-B50B-00E0006700B4}">
+          <x14:cfRule type="cellIs" priority="28" operator="lessThan" stopIfTrue="1" id="{00FF00EA-0054-494D-91F8-009B00790028}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10589,7 +10589,7 @@
           <xm:sqref>BE10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="27" operator="between" stopIfTrue="1" id="{006000CA-00FF-4CA8-A2A5-00F600600021}">
+          <x14:cfRule type="cellIs" priority="27" operator="between" stopIfTrue="1" id="{002A0077-00EA-4A35-B252-00E800670039}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10609,7 +10609,7 @@
           <xm:sqref>BC10:BD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="26" operator="greaterThan" stopIfTrue="1" id="{000300D4-0044-429B-943F-0097005A00B8}">
+          <x14:cfRule type="cellIs" priority="26" operator="greaterThan" stopIfTrue="1" id="{002800D4-00ED-4F2A-AEFC-007B001D009A}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10628,7 +10628,7 @@
           <xm:sqref>BC10:BD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="25" operator="lessThan" stopIfTrue="1" id="{00FD0079-0093-4449-AFB9-007300690094}">
+          <x14:cfRule type="cellIs" priority="25" operator="lessThan" stopIfTrue="1" id="{00F90094-00E7-43D0-B08E-00C5002000FE}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10647,7 +10647,7 @@
           <xm:sqref>BC10:BD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="24" operator="between" stopIfTrue="1" id="{00DE0027-00D5-4ABD-9334-0085005900FB}">
+          <x14:cfRule type="cellIs" priority="24" operator="between" stopIfTrue="1" id="{00BD00AD-007B-4984-B2C9-009100300060}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10667,7 +10667,7 @@
           <xm:sqref>AM10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="23" operator="greaterThan" stopIfTrue="1" id="{00D5003E-005A-4D1C-91A0-008F001D0036}">
+          <x14:cfRule type="cellIs" priority="23" operator="greaterThan" stopIfTrue="1" id="{00190042-004A-4B7F-A670-00D2009500E2}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10686,7 +10686,7 @@
           <xm:sqref>AM10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="22" operator="lessThan" stopIfTrue="1" id="{00AD0052-0094-4A19-B918-00C000D500B4}">
+          <x14:cfRule type="cellIs" priority="22" operator="lessThan" stopIfTrue="1" id="{00A800B9-0000-41AA-895A-002C00BD0067}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10705,7 +10705,7 @@
           <xm:sqref>AM10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="21" operator="between" stopIfTrue="1" id="{00540045-00A2-4E59-B3DD-002900C600FE}">
+          <x14:cfRule type="cellIs" priority="21" operator="between" stopIfTrue="1" id="{00C600E9-0074-4765-85FB-00DF007E0020}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10725,7 +10725,7 @@
           <xm:sqref>AP10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="20" operator="greaterThan" stopIfTrue="1" id="{00D50097-00F1-439F-B8CD-00CA00CA00FC}">
+          <x14:cfRule type="cellIs" priority="20" operator="greaterThan" stopIfTrue="1" id="{00D800E5-0021-4EF5-A64B-0074007A00A4}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10744,7 +10744,7 @@
           <xm:sqref>AP10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="19" operator="lessThan" stopIfTrue="1" id="{00340000-00F1-4B80-B5FE-00B30026000E}">
+          <x14:cfRule type="cellIs" priority="19" operator="lessThan" stopIfTrue="1" id="{0068004F-0032-4201-A589-00F000B700B6}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10763,7 +10763,7 @@
           <xm:sqref>AP10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="18" operator="between" stopIfTrue="1" id="{0053008E-00D6-4855-BD62-008400C000C7}">
+          <x14:cfRule type="cellIs" priority="18" operator="between" stopIfTrue="1" id="{009B0042-00B3-477B-BF6C-00FA007B00EF}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10783,7 +10783,7 @@
           <xm:sqref>AO10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="17" operator="greaterThan" stopIfTrue="1" id="{0055004A-00DF-4259-9F90-009A00B7009C}">
+          <x14:cfRule type="cellIs" priority="17" operator="greaterThan" stopIfTrue="1" id="{0039005D-0075-4395-A4DC-008C00210032}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10802,7 +10802,7 @@
           <xm:sqref>AO10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="16" operator="lessThan" stopIfTrue="1" id="{0014001E-00A5-4405-8B10-000E001400A9}">
+          <x14:cfRule type="cellIs" priority="16" operator="lessThan" stopIfTrue="1" id="{00A900BD-0046-43F2-93C2-006100D100F0}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10821,7 +10821,7 @@
           <xm:sqref>AO10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="15" operator="between" stopIfTrue="1" id="{008A0081-003F-40C3-93D2-003F00D200CC}">
+          <x14:cfRule type="cellIs" priority="15" operator="between" stopIfTrue="1" id="{00CE0068-002E-4DDF-BB01-00DF00AD00FE}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10841,7 +10841,7 @@
           <xm:sqref>AN10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="14" operator="greaterThan" stopIfTrue="1" id="{007800A7-00F9-4BDB-9C3C-006B000500FF}">
+          <x14:cfRule type="cellIs" priority="14" operator="greaterThan" stopIfTrue="1" id="{004700C1-00AA-4515-9C56-0068006200AA}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10860,7 +10860,7 @@
           <xm:sqref>AN10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="13" operator="lessThan" stopIfTrue="1" id="{00CB005F-00B8-4D21-9028-006E004200B0}">
+          <x14:cfRule type="cellIs" priority="13" operator="lessThan" stopIfTrue="1" id="{00B2009A-003C-44C2-A8FB-00DF004D00CB}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10879,7 +10879,7 @@
           <xm:sqref>AN10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="12" operator="between" stopIfTrue="1" id="{00DF00E6-0032-4E13-9DA3-0014006D00CD}">
+          <x14:cfRule type="cellIs" priority="12" operator="between" stopIfTrue="1" id="{004000A9-0055-4B42-9712-009800FC000E}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10899,7 +10899,7 @@
           <xm:sqref>AA10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="11" operator="greaterThan" stopIfTrue="1" id="{00640052-00AC-4C64-B953-002B00250004}">
+          <x14:cfRule type="cellIs" priority="11" operator="greaterThan" stopIfTrue="1" id="{006100B1-00A8-45B7-B276-004000880003}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10918,7 +10918,7 @@
           <xm:sqref>AA10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="10" operator="lessThan" stopIfTrue="1" id="{00660005-0060-44B6-8ABE-00B800BD00B1}">
+          <x14:cfRule type="cellIs" priority="10" operator="lessThan" stopIfTrue="1" id="{008E0067-0047-4CC3-A623-00860019000A}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10937,7 +10937,7 @@
           <xm:sqref>AA10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="9" operator="between" stopIfTrue="1" id="{00F8008E-00CF-492B-A0DA-0070007300A2}">
+          <x14:cfRule type="cellIs" priority="9" operator="between" stopIfTrue="1" id="{00900009-008A-4882-B0EB-00EF00460094}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -10957,7 +10957,7 @@
           <xm:sqref>AD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="8" operator="greaterThan" stopIfTrue="1" id="{00D9002E-00B1-45D5-BACD-00CB00A2003C}">
+          <x14:cfRule type="cellIs" priority="8" operator="greaterThan" stopIfTrue="1" id="{00FA0009-003A-47F7-BBC9-009100A10086}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -10976,7 +10976,7 @@
           <xm:sqref>AD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="7" operator="lessThan" stopIfTrue="1" id="{00B8009F-00F4-4606-BEF2-00A1005A00D7}">
+          <x14:cfRule type="cellIs" priority="7" operator="lessThan" stopIfTrue="1" id="{00FB00DB-008D-4DF1-BF84-00DC004900C3}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -10995,7 +10995,7 @@
           <xm:sqref>AD10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="between" stopIfTrue="1" id="{005A00CE-004A-49B8-A679-0045005800B1}">
+          <x14:cfRule type="cellIs" priority="6" operator="between" stopIfTrue="1" id="{003D00F8-0081-45A9-AEEB-001A006100A6}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -11015,7 +11015,7 @@
           <xm:sqref>AC10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="greaterThan" stopIfTrue="1" id="{004A00E1-00AC-430D-BD01-001D003E00BD}">
+          <x14:cfRule type="cellIs" priority="5" operator="greaterThan" stopIfTrue="1" id="{00F700DA-009E-4D71-BC29-009400E700C7}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -11034,7 +11034,7 @@
           <xm:sqref>AC10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="lessThan" stopIfTrue="1" id="{003400FD-00C8-455D-9F05-009900AC004E}">
+          <x14:cfRule type="cellIs" priority="4" operator="lessThan" stopIfTrue="1" id="{00690030-00C9-46A6-BDA0-00C0006B003F}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>
@@ -11053,7 +11053,7 @@
           <xm:sqref>AC10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="between" stopIfTrue="1" id="{004400E0-000F-4792-9A7C-0070009E0022}">
+          <x14:cfRule type="cellIs" priority="3" operator="between" stopIfTrue="1" id="{004100FE-00BE-409A-ACB2-00E3000D0012}">
             <xm:f>0.65900000000000003</xm:f>
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
@@ -11073,7 +11073,7 @@
           <xm:sqref>AB10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="greaterThan" stopIfTrue="1" id="{002C0079-007A-4D6F-935D-00AC00250067}">
+          <x14:cfRule type="cellIs" priority="2" operator="greaterThan" stopIfTrue="1" id="{00610006-00A2-4C9A-9F92-00AA0018001F}">
             <xm:f>0.85899999999999999</xm:f>
             <x14:dxf>
               <font>
@@ -11092,7 +11092,7 @@
           <xm:sqref>AB10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="lessThan" stopIfTrue="1" id="{00910010-00F6-4443-B24A-0015009700B9}">
+          <x14:cfRule type="cellIs" priority="1" operator="lessThan" stopIfTrue="1" id="{007800F3-0086-4F38-9042-00AB009A008A}">
             <xm:f>0.66000000000000003</xm:f>
             <x14:dxf>
               <font>

</xml_diff>